<commit_message>
added covid 19 infograph
</commit_message>
<xml_diff>
--- a/papers/04TH/classdescription/class_marks.xlsx
+++ b/papers/04TH/classdescription/class_marks.xlsx
@@ -15,12 +15,12 @@
     <sheet name="grade dist" sheetId="5" r:id="rId1"/>
     <sheet name="table " sheetId="1" r:id="rId2"/>
     <sheet name="student_total_marks_rankings" sheetId="6" r:id="rId3"/>
-    <sheet name="student ranking graph" sheetId="4" r:id="rId4"/>
-    <sheet name="grades_bands" sheetId="3" r:id="rId5"/>
+    <sheet name="grades_bands" sheetId="3" r:id="rId4"/>
+    <sheet name="student ranking graph" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
   <si>
     <r>
       <rPr>
@@ -1013,15 +1013,72 @@
   <si>
     <t>Grade</t>
   </si>
+  <si>
+    <t>Assn weighted score</t>
+  </si>
+  <si>
+    <t>mid_wt_score</t>
+  </si>
+  <si>
+    <t>final_wt_score</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>70-75</t>
+  </si>
+  <si>
+    <t>73-78</t>
+  </si>
+  <si>
+    <t>73-79</t>
+  </si>
+  <si>
+    <t>73-80</t>
+  </si>
+  <si>
+    <t>77-81</t>
+  </si>
+  <si>
+    <t>77-82</t>
+  </si>
+  <si>
+    <t>80-86</t>
+  </si>
+  <si>
+    <t>80-87</t>
+  </si>
+  <si>
+    <t>80-88</t>
+  </si>
+  <si>
+    <t>80-89</t>
+  </si>
+  <si>
+    <t>85-91</t>
+  </si>
+  <si>
+    <t>85-92</t>
+  </si>
+  <si>
+    <t>85-93</t>
+  </si>
+  <si>
+    <t>85-94</t>
+  </si>
+  <si>
+    <t>73--77</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,14 +1186,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1177,9 +1226,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1189,11 +1237,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,33 +1348,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="84000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="20000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1529,11 +1559,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="1094304416"/>
-        <c:axId val="1094300608"/>
+        <c:axId val="-1595216608"/>
+        <c:axId val="-1595209536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1094304416"/>
+        <c:axId val="-1595216608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1094300608"/>
+        <c:crossAx val="-1595209536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1094300608"/>
+        <c:axId val="-1595209536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1619,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1094304416"/>
+        <c:crossAx val="-1595216608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2902,11 +2932,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="753956656"/>
-        <c:axId val="753956112"/>
+        <c:axId val="-1595204640"/>
+        <c:axId val="-1595207904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="753956656"/>
+        <c:axId val="-1595204640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2948,7 +2978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753956112"/>
+        <c:crossAx val="-1595207904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2956,7 +2986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="753956112"/>
+        <c:axId val="-1595207904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3006,7 +3036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753956656"/>
+        <c:crossAx val="-1595204640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3336,46 +3366,46 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>92.333333333333329</c:v>
+                  <c:v>91.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.666666666666664</c:v>
+                  <c:v>54.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.333333333333329</c:v>
+                  <c:v>74.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>74.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71</c:v>
+                  <c:v>71.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83</c:v>
+                  <c:v>80.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76</c:v>
+                  <c:v>75.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>56.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.666666666666671</c:v>
+                  <c:v>81.05</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70</c:v>
+                  <c:v>69.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59.666666666666664</c:v>
+                  <c:v>66.550000000000011</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>62.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.333333333333336</c:v>
+                  <c:v>54.95</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>66.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3391,11 +3421,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="753955024"/>
-        <c:axId val="753954480"/>
+        <c:axId val="-1595205184"/>
+        <c:axId val="-1595206272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="753955024"/>
+        <c:axId val="-1595205184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3433,7 +3463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753954480"/>
+        <c:crossAx val="-1595206272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3441,7 +3471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="753954480"/>
+        <c:axId val="-1595206272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3451,7 +3481,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="753955024"/>
+        <c:crossAx val="-1595205184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5372,7 +5402,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Onyango Ogolla" refreshedDate="44534.669238773145" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="14">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J15" sheet="table "/>
+    <worksheetSource ref="A1:M15" sheet="table "/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="First name" numFmtId="0">
@@ -5399,7 +5429,7 @@
     <cacheField name="AVERAGE %" numFmtId="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="55.333333333333336" maxValue="92.333333333333329"/>
     </cacheField>
-    <cacheField name="grade_bands" numFmtId="174">
+    <cacheField name="grade_bands" numFmtId="164">
       <sharedItems/>
     </cacheField>
     <cacheField name="GRADE" numFmtId="0">
@@ -5595,7 +5625,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Grade">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Grade">
   <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -5953,11 +5983,11 @@
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
@@ -5965,58 +5995,58 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>14</v>
       </c>
     </row>
@@ -6028,61 +6058,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="L1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="M1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
@@ -6094,30 +6136,42 @@
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
+        <f>D2*0.2</f>
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>85</v>
       </c>
-      <c r="F2">
+      <c r="G2" s="10">
+        <f>F2*0.35</f>
+        <v>29.749999999999996</v>
+      </c>
+      <c r="H2">
         <v>92</v>
       </c>
-      <c r="G2" s="11">
-        <f>SUM(D2:F2)</f>
-        <v>277</v>
-      </c>
-      <c r="H2" s="12">
-        <f>AVERAGE(D2:F2)</f>
-        <v>92.333333333333329</v>
-      </c>
-      <c r="I2" s="11" t="str">
-        <f>IF(H2&gt;=90,"A+",IF(H2&gt;=85,"A",IF(H2&gt;=80,"A-",IF(H2&gt;=77,"B+",IF(H2&gt;=73,"B+",IF(H2&gt;=70,"B",IF(H2&gt;=70,"B-",IF(H2&gt;=60,"C",IF(H2&lt;60,"F")))))))))</f>
+      <c r="I2" s="10">
+        <f>H2*0.45</f>
+        <v>41.4</v>
+      </c>
+      <c r="J2" s="12">
+        <f>E2+G2+I2</f>
+        <v>91.15</v>
+      </c>
+      <c r="K2" s="12">
+        <f>AVERAGE(E2+G2+I2)</f>
+        <v>91.15</v>
+      </c>
+      <c r="L2" s="9" t="str">
+        <f>IF(K2&gt;=90,"A+",IF(K2&gt;=85,"A",IF(K2&gt;=80,"A-",IF(K2&gt;=77,"B+",IF(K2&gt;=73,"B+",IF(K2&gt;=70,"B",IF(K2&gt;=70,"B-",IF(K2&gt;=60,"C",IF(K2&lt;60,"F")))))))))</f>
         <v>A+</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="M2" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -6129,30 +6183,42 @@
       <c r="D3">
         <v>87</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E15" si="0">D3*0.2</f>
+        <v>17.400000000000002</v>
+      </c>
+      <c r="F3">
         <v>55</v>
       </c>
-      <c r="F3">
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G15" si="1">F3*0.35</f>
+        <v>19.25</v>
+      </c>
+      <c r="H3">
         <v>40</v>
       </c>
-      <c r="G3" s="11">
-        <f t="shared" ref="G3:G15" si="0">SUM(D3:F3)</f>
-        <v>182</v>
-      </c>
-      <c r="H3" s="12">
-        <f t="shared" ref="H3:H15" si="1">AVERAGE(D3:F3)</f>
-        <v>60.666666666666664</v>
-      </c>
-      <c r="I3" s="11" t="str">
-        <f>IF(H3&gt;=90,"A+",IF(H3&gt;=85,"A",IF(H3&gt;=80,"A-",IF(H3&gt;=77,"B+",IF(H3&gt;=73,"B+",IF(H3&gt;=70,"B",IF(H3&gt;=70,"B-",IF(H3&gt;=60,"C",IF(H3&lt;60,"F")))))))))</f>
-        <v>C</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="10">
+        <f t="shared" ref="I3:I15" si="2">H3*0.45</f>
+        <v>18</v>
+      </c>
+      <c r="J3" s="12">
+        <f t="shared" ref="J3:J15" si="3">E3+G3+I3</f>
+        <v>54.650000000000006</v>
+      </c>
+      <c r="K3" s="12">
+        <f t="shared" ref="K3:K15" si="4">AVERAGE(E3+G3+I3)</f>
+        <v>54.650000000000006</v>
+      </c>
+      <c r="L3" s="9" t="str">
+        <f>IF(K3&gt;=90,"A+",IF(K3&gt;=85,"A",IF(K3&gt;=80,"A-",IF(K3&gt;=77,"B+",IF(K3&gt;=73,"B+",IF(K3&gt;=70,"B",IF(K3&gt;=70,"B-",IF(K3&gt;=60,"C",IF(K3&lt;60,"F")))))))))</f>
+        <v>F</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
@@ -6164,30 +6230,42 @@
       <c r="D4">
         <v>45</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F4">
         <v>88</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="10">
+        <f t="shared" si="1"/>
+        <v>30.799999999999997</v>
+      </c>
+      <c r="H4">
         <v>78</v>
       </c>
-      <c r="G4" s="11">
-        <f t="shared" si="0"/>
-        <v>211</v>
-      </c>
-      <c r="H4" s="12">
-        <f t="shared" si="1"/>
-        <v>70.333333333333329</v>
-      </c>
-      <c r="I4" s="11" t="str">
-        <f>IF(H4&gt;=90,"A+",IF(H4&gt;=85,"A",IF(H4&gt;=80,"A-",IF(H4&gt;=77,"B+",IF(H4&gt;=73,"B+",IF(H4&gt;=70,"B",IF(H4&gt;=70,"B-",IF(H4&gt;=60,"C",IF(H4&lt;60,"F")))))))))</f>
-        <v>B</v>
-      </c>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="10">
+        <f t="shared" si="2"/>
+        <v>35.1</v>
+      </c>
+      <c r="J4" s="12">
+        <f t="shared" si="3"/>
+        <v>74.900000000000006</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" si="4"/>
+        <v>74.900000000000006</v>
+      </c>
+      <c r="L4" s="9" t="str">
+        <f>IF(K4&gt;=90,"A+",IF(K4&gt;=85,"A",IF(K4&gt;=80,"A-",IF(K4&gt;=77,"B+",IF(K4&gt;=73,"B+",IF(K4&gt;=70,"B",IF(K4&gt;=70,"B-",IF(K4&gt;=60,"C",IF(K4&lt;60,"F")))))))))</f>
+        <v>B+</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
@@ -6199,31 +6277,42 @@
       <c r="D5">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>76</v>
       </c>
-      <c r="F5">
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
+        <v>26.599999999999998</v>
+      </c>
+      <c r="H5">
         <v>84</v>
       </c>
-      <c r="G5" s="11">
-        <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
-      <c r="H5" s="12">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="I5" s="11" t="str">
-        <f>IF(H5&gt;=90,"A+",IF(H5&gt;=85,"A",IF(H5&gt;=80,"A-",IF(H5&gt;=77,"B+",IF(H5&gt;=73,"B+",IF(H5&gt;=70,"B",IF(H5&gt;=70,"B-",IF(H5&gt;=60,"C",IF(H5&lt;60,"F")))))))))</f>
-        <v>B</v>
-      </c>
-      <c r="J5" s="13" t="str">
-        <f>VLOOKUP($H$2:$H$15,grades_bands!$A$2:$B$45,2,0)</f>
-        <v>70-73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="I5" s="10">
+        <f t="shared" si="2"/>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" si="3"/>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" si="4"/>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="L5" s="9" t="str">
+        <f>IF(K5&gt;=90,"A+",IF(K5&gt;=85,"A",IF(K5&gt;=80,"A-",IF(K5&gt;=77,"B+",IF(K5&gt;=73,"B+",IF(K5&gt;=70,"B",IF(K5&gt;=70,"B-",IF(K5&gt;=60,"C",IF(K5&lt;60,"F")))))))))</f>
+        <v>B+</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -6235,30 +6324,42 @@
       <c r="D6">
         <v>74</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>14.8</v>
+      </c>
+      <c r="F6">
         <v>55</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="10">
+        <f t="shared" si="1"/>
+        <v>19.25</v>
+      </c>
+      <c r="H6">
         <v>84</v>
       </c>
-      <c r="G6" s="11">
-        <f t="shared" si="0"/>
-        <v>213</v>
-      </c>
-      <c r="H6" s="12">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="I6" s="11" t="str">
-        <f>IF(H6&gt;=90,"A+",IF(H6&gt;=85,"A",IF(H6&gt;=80,"A-",IF(H6&gt;=77,"B+",IF(H6&gt;=73,"B+",IF(H6&gt;=70,"B",IF(H6&gt;=70,"B-",IF(H6&gt;=60,"C",IF(H6&lt;60,"F")))))))))</f>
+      <c r="I6" s="10">
+        <f t="shared" si="2"/>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="J6" s="12">
+        <f t="shared" si="3"/>
+        <v>71.849999999999994</v>
+      </c>
+      <c r="K6" s="12">
+        <f t="shared" si="4"/>
+        <v>71.849999999999994</v>
+      </c>
+      <c r="L6" s="9" t="str">
+        <f>IF(K6&gt;=90,"A+",IF(K6&gt;=85,"A",IF(K6&gt;=80,"A-",IF(K6&gt;=77,"B+",IF(K6&gt;=73,"B+",IF(K6&gt;=70,"B",IF(K6&gt;=70,"B-",IF(K6&gt;=60,"C",IF(K6&lt;60,"F")))))))))</f>
         <v>B</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="M6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -6270,30 +6371,42 @@
       <c r="D7">
         <v>98</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="F7">
         <v>71</v>
       </c>
-      <c r="F7">
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>24.849999999999998</v>
+      </c>
+      <c r="H7">
         <v>80</v>
       </c>
-      <c r="G7" s="11">
-        <f t="shared" si="0"/>
-        <v>249</v>
-      </c>
-      <c r="H7" s="12">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="I7" s="11" t="str">
-        <f>IF(H7&gt;=90,"A+",IF(H7&gt;=85,"A",IF(H7&gt;=80,"A-",IF(H7&gt;=77,"B+",IF(H7&gt;=73,"B+",IF(H7&gt;=70,"B",IF(H7&gt;=70,"B-",IF(H7&gt;=60,"C",IF(H7&lt;60,"F")))))))))</f>
+      <c r="I7" s="10">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="3"/>
+        <v>80.45</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="4"/>
+        <v>80.45</v>
+      </c>
+      <c r="L7" s="9" t="str">
+        <f>IF(K7&gt;=90,"A+",IF(K7&gt;=85,"A",IF(K7&gt;=80,"A-",IF(K7&gt;=77,"B+",IF(K7&gt;=73,"B+",IF(K7&gt;=70,"B",IF(K7&gt;=70,"B-",IF(K7&gt;=60,"C",IF(K7&lt;60,"F")))))))))</f>
         <v>A-</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="M7" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -6305,31 +6418,42 @@
       <c r="D8">
         <v>78</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="F8">
         <v>74</v>
       </c>
-      <c r="F8">
+      <c r="G8" s="10">
+        <f t="shared" si="1"/>
+        <v>25.9</v>
+      </c>
+      <c r="H8">
         <v>76</v>
       </c>
-      <c r="G8" s="11">
-        <f t="shared" si="0"/>
-        <v>228</v>
-      </c>
-      <c r="H8" s="12">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="I8" s="11" t="str">
-        <f>IF(H8&gt;=90,"A+",IF(H8&gt;=85,"A",IF(H8&gt;=80,"A-",IF(H8&gt;=77,"B+",IF(H8&gt;=73,"B+",IF(H8&gt;=70,"B",IF(H8&gt;=70,"B-",IF(H8&gt;=60,"C",IF(H8&lt;60,"F")))))))))</f>
+      <c r="I8" s="10">
+        <f t="shared" si="2"/>
+        <v>34.200000000000003</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="3"/>
+        <v>75.7</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="4"/>
+        <v>75.7</v>
+      </c>
+      <c r="L8" s="9" t="str">
+        <f>IF(K8&gt;=90,"A+",IF(K8&gt;=85,"A",IF(K8&gt;=80,"A-",IF(K8&gt;=77,"B+",IF(K8&gt;=73,"B+",IF(K8&gt;=70,"B",IF(K8&gt;=70,"B-",IF(K8&gt;=60,"C",IF(K8&lt;60,"F")))))))))</f>
         <v>B+</v>
       </c>
-      <c r="J8" s="13" t="str">
-        <f>VLOOKUP($H$2:$H$15,grades_bands!$A$2:$B$45,2,0)</f>
-        <v>73-77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="M8" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
@@ -6341,31 +6465,42 @@
       <c r="D9">
         <v>54</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+      <c r="F9">
         <v>59</v>
       </c>
-      <c r="F9">
+      <c r="G9" s="10">
+        <f t="shared" si="1"/>
+        <v>20.65</v>
+      </c>
+      <c r="H9">
         <v>55</v>
       </c>
-      <c r="G9" s="11">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="H9" s="12">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="I9" s="11" t="str">
-        <f>IF(H9&gt;=90,"A+",IF(H9&gt;=85,"A",IF(H9&gt;=80,"A-",IF(H9&gt;=77,"B+",IF(H9&gt;=73,"B+",IF(H9&gt;=70,"B",IF(H9&gt;=70,"B-",IF(H9&gt;=60,"C",IF(H9&lt;60,"F")))))))))</f>
+      <c r="I9" s="10">
+        <f t="shared" si="2"/>
+        <v>24.75</v>
+      </c>
+      <c r="J9" s="12">
+        <f t="shared" si="3"/>
+        <v>56.2</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="4"/>
+        <v>56.2</v>
+      </c>
+      <c r="L9" s="9" t="str">
+        <f>IF(K9&gt;=90,"A+",IF(K9&gt;=85,"A",IF(K9&gt;=80,"A-",IF(K9&gt;=77,"B+",IF(K9&gt;=73,"B+",IF(K9&gt;=70,"B",IF(K9&gt;=70,"B-",IF(K9&gt;=60,"C",IF(K9&lt;60,"F")))))))))</f>
         <v>F</v>
       </c>
-      <c r="J9" s="13" t="str">
-        <f>VLOOKUP($H$2:$H$15,grades_bands!$A$2:$B$45,2,0)</f>
-        <v>0-59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="M9" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -6377,30 +6512,42 @@
       <c r="D10">
         <v>88</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F10">
         <v>72</v>
       </c>
-      <c r="F10">
+      <c r="G10" s="10">
+        <f t="shared" si="1"/>
+        <v>25.2</v>
+      </c>
+      <c r="H10">
         <v>85</v>
       </c>
-      <c r="G10" s="11">
-        <f t="shared" si="0"/>
-        <v>245</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" si="1"/>
-        <v>81.666666666666671</v>
-      </c>
-      <c r="I10" s="11" t="str">
-        <f>IF(H10&gt;=90,"A+",IF(H10&gt;=85,"A",IF(H10&gt;=80,"A-",IF(H10&gt;=77,"B+",IF(H10&gt;=73,"B+",IF(H10&gt;=70,"B",IF(H10&gt;=70,"B-",IF(H10&gt;=60,"C",IF(H10&lt;60,"F")))))))))</f>
+      <c r="I10" s="10">
+        <f t="shared" si="2"/>
+        <v>38.25</v>
+      </c>
+      <c r="J10" s="12">
+        <f t="shared" si="3"/>
+        <v>81.05</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="4"/>
+        <v>81.05</v>
+      </c>
+      <c r="L10" s="9" t="str">
+        <f>IF(K10&gt;=90,"A+",IF(K10&gt;=85,"A",IF(K10&gt;=80,"A-",IF(K10&gt;=77,"B+",IF(K10&gt;=73,"B+",IF(K10&gt;=70,"B",IF(K10&gt;=70,"B-",IF(K10&gt;=60,"C",IF(K10&lt;60,"F")))))))))</f>
         <v>A-</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="M10" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
@@ -6412,31 +6559,42 @@
       <c r="D11">
         <v>73</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="9">
+        <f t="shared" si="0"/>
+        <v>14.600000000000001</v>
+      </c>
+      <c r="F11">
         <v>65</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="10">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
+      </c>
+      <c r="H11">
         <v>72</v>
       </c>
-      <c r="G11" s="11">
-        <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
-      <c r="H11" s="12">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="I11" s="11" t="str">
-        <f>IF(H11&gt;=90,"A+",IF(H11&gt;=85,"A",IF(H11&gt;=80,"A-",IF(H11&gt;=77,"B+",IF(H11&gt;=73,"B+",IF(H11&gt;=70,"B",IF(H11&gt;=70,"B-",IF(H11&gt;=60,"C",IF(H11&lt;60,"F")))))))))</f>
-        <v>B</v>
-      </c>
-      <c r="J11" s="13" t="str">
-        <f>VLOOKUP($H$2:$H$15,grades_bands!$A$2:$B$45,2,0)</f>
-        <v>70-73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="I11" s="10">
+        <f t="shared" si="2"/>
+        <v>32.4</v>
+      </c>
+      <c r="J11" s="12">
+        <f t="shared" si="3"/>
+        <v>69.75</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="4"/>
+        <v>69.75</v>
+      </c>
+      <c r="L11" s="9" t="str">
+        <f>IF(K11&gt;=90,"A+",IF(K11&gt;=85,"A",IF(K11&gt;=80,"A-",IF(K11&gt;=77,"B+",IF(K11&gt;=73,"B+",IF(K11&gt;=70,"B",IF(K11&gt;=70,"B-",IF(K11&gt;=60,"C",IF(K11&lt;60,"F")))))))))</f>
+        <v>C</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -6448,30 +6606,42 @@
       <c r="D12">
         <v>30</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F12">
         <v>65</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="10">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
+      </c>
+      <c r="H12">
         <v>84</v>
       </c>
-      <c r="G12" s="11">
-        <f t="shared" si="0"/>
-        <v>179</v>
-      </c>
-      <c r="H12" s="12">
-        <f t="shared" si="1"/>
-        <v>59.666666666666664</v>
-      </c>
-      <c r="I12" s="11" t="str">
-        <f>IF(H12&gt;=90,"A+",IF(H12&gt;=85,"A",IF(H12&gt;=80,"A-",IF(H12&gt;=77,"B+",IF(H12&gt;=73,"B+",IF(H12&gt;=70,"B",IF(H12&gt;=70,"B-",IF(H12&gt;=60,"C",IF(H12&lt;60,"F")))))))))</f>
-        <v>F</v>
-      </c>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="10">
+        <f t="shared" si="2"/>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="3"/>
+        <v>66.550000000000011</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="4"/>
+        <v>66.550000000000011</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f>IF(K12&gt;=90,"A+",IF(K12&gt;=85,"A",IF(K12&gt;=80,"A-",IF(K12&gt;=77,"B+",IF(K12&gt;=73,"B+",IF(K12&gt;=70,"B",IF(K12&gt;=70,"B-",IF(K12&gt;=60,"C",IF(K12&lt;60,"F")))))))))</f>
+        <v>C</v>
+      </c>
+      <c r="M12" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
@@ -6483,31 +6653,42 @@
       <c r="D13">
         <v>63</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
+        <v>12.600000000000001</v>
+      </c>
+      <c r="F13">
         <v>78</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="10">
+        <f t="shared" si="1"/>
+        <v>27.299999999999997</v>
+      </c>
+      <c r="H13">
         <v>51</v>
       </c>
-      <c r="G13" s="11">
-        <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-      <c r="H13" s="12">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="I13" s="11" t="str">
-        <f>IF(H13&gt;=90,"A+",IF(H13&gt;=85,"A",IF(H13&gt;=80,"A-",IF(H13&gt;=77,"B+",IF(H13&gt;=73,"B+",IF(H13&gt;=70,"B",IF(H13&gt;=70,"B-",IF(H13&gt;=60,"C",IF(H13&lt;60,"F")))))))))</f>
+      <c r="I13" s="10">
+        <f t="shared" si="2"/>
+        <v>22.95</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" si="3"/>
+        <v>62.849999999999994</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="4"/>
+        <v>62.849999999999994</v>
+      </c>
+      <c r="L13" s="9" t="str">
+        <f>IF(K13&gt;=90,"A+",IF(K13&gt;=85,"A",IF(K13&gt;=80,"A-",IF(K13&gt;=77,"B+",IF(K13&gt;=73,"B+",IF(K13&gt;=70,"B",IF(K13&gt;=70,"B-",IF(K13&gt;=60,"C",IF(K13&lt;60,"F")))))))))</f>
         <v>C</v>
       </c>
-      <c r="J13" s="13" t="str">
-        <f>VLOOKUP($H$2:$H$15,grades_bands!$A$2:$B$45,2,0)</f>
-        <v>60-70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="M13" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
@@ -6519,30 +6700,42 @@
       <c r="D14">
         <v>61</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="9">
+        <f t="shared" si="0"/>
+        <v>12.200000000000001</v>
+      </c>
+      <c r="F14">
         <v>45</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="10">
+        <f t="shared" si="1"/>
+        <v>15.749999999999998</v>
+      </c>
+      <c r="H14">
         <v>60</v>
       </c>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>166</v>
-      </c>
-      <c r="H14" s="12">
-        <f t="shared" si="1"/>
-        <v>55.333333333333336</v>
-      </c>
-      <c r="I14" s="11" t="str">
-        <f>IF(H14&gt;=90,"A+",IF(H14&gt;=85,"A",IF(H14&gt;=80,"A-",IF(H14&gt;=77,"B+",IF(H14&gt;=73,"B+",IF(H14&gt;=70,"B",IF(H14&gt;=70,"B-",IF(H14&gt;=60,"C",IF(H14&lt;60,"F")))))))))</f>
+      <c r="I14" s="10">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="3"/>
+        <v>54.95</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="4"/>
+        <v>54.95</v>
+      </c>
+      <c r="L14" s="9" t="str">
+        <f>IF(K14&gt;=90,"A+",IF(K14&gt;=85,"A",IF(K14&gt;=80,"A-",IF(K14&gt;=77,"B+",IF(K14&gt;=73,"B+",IF(K14&gt;=70,"B",IF(K14&gt;=70,"B-",IF(K14&gt;=60,"C",IF(K14&lt;60,"F")))))))))</f>
         <v>F</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="M14" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
@@ -6554,58 +6747,51 @@
       <c r="D15">
         <v>55</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F15">
         <v>78</v>
       </c>
-      <c r="F15">
+      <c r="G15" s="10">
+        <f t="shared" si="1"/>
+        <v>27.299999999999997</v>
+      </c>
+      <c r="H15">
         <v>62</v>
       </c>
-      <c r="G15" s="11">
-        <f t="shared" si="0"/>
-        <v>195</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="I15" s="11" t="str">
-        <f>IF(H15&gt;=90,"A+",IF(H15&gt;=85,"A",IF(H15&gt;=80,"A-",IF(H15&gt;=77,"B+",IF(H15&gt;=73,"B+",IF(H15&gt;=70,"B",IF(H15&gt;=70,"B-",IF(H15&gt;=60,"C",IF(H15&lt;60,"F")))))))))</f>
+      <c r="I15" s="10">
+        <f t="shared" si="2"/>
+        <v>27.900000000000002</v>
+      </c>
+      <c r="J15" s="12">
+        <f t="shared" si="3"/>
+        <v>66.2</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="4"/>
+        <v>66.2</v>
+      </c>
+      <c r="L15" s="9" t="str">
+        <f>IF(K15&gt;=90,"A+",IF(K15&gt;=85,"A",IF(K15&gt;=80,"A-",IF(K15&gt;=77,"B+",IF(K15&gt;=73,"B+",IF(K15&gt;=70,"B",IF(K15&gt;=70,"B-",IF(K15&gt;=60,"C",IF(K15&lt;60,"F")))))))))</f>
         <v>C</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="M15" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="9">
-        <f>SUM(D2:D15)</f>
-        <v>956</v>
-      </c>
-      <c r="E17" s="9">
-        <f t="shared" ref="E17:H17" si="2">SUM(E2:E15)</f>
-        <v>966</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" si="2"/>
-        <v>1003</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" si="2"/>
-        <v>2925</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="shared" si="2"/>
-        <v>974.99999999999989</v>
-      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
     </row>
   </sheetData>
   <sortState ref="A2:F15">
@@ -6620,21 +6806,21 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6758,24 +6944,851 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="14"/>
+    <col min="2" max="2" width="11.42578125" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>19</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>21</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>27</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>28</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>30</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>31</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>32</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>33</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>34</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>35</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>36</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>37</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>38</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>39</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>40</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>41</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>42</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>43</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>44</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>45</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>46</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>47</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>48</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>49</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>50</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>51</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>52</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>53</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <v>54</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>55</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <v>56</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <v>57</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>58</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>59</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>60</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>61</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>62</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>63</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>64</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>65</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>66</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>67</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <v>68</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
+        <v>69</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <v>70</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <v>71</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <v>72</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <v>73</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>74</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <v>75</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>76</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
+        <v>77</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
+        <v>78</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <v>79</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
+        <v>80</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="14">
+        <v>81</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="14">
+        <v>82</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="14">
+        <v>83</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="14">
+        <v>84</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="14">
+        <v>85</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="14">
+        <v>86</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="14">
+        <v>87</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="14">
+        <v>88</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="14">
+        <v>89</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="14">
+        <v>90</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="14">
+        <v>91</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="14">
+        <v>92</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="14">
+        <v>93</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="14">
+        <v>94</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="14">
+        <v>95</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="14">
+        <v>96</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="14">
+        <v>97</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="14">
+        <v>98</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="14">
+        <v>99</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="14">
+        <v>100</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6783,494 +7796,116 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3">
-        <v>92.333333333333329</v>
+      <c r="B2" s="2">
+        <v>91.15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>60.666666666666664</v>
+      <c r="B3" s="2">
+        <v>54.650000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3">
-        <v>70.333333333333329</v>
+      <c r="B4" s="2">
+        <v>74.900000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3">
-        <v>70</v>
+      <c r="B5" s="2">
+        <v>74.400000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
-        <v>71</v>
+      <c r="B6" s="2">
+        <v>71.849999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3">
-        <v>83</v>
+      <c r="B7" s="2">
+        <v>80.45</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3">
-        <v>76</v>
+      <c r="B8" s="2">
+        <v>75.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3">
-        <v>56</v>
+      <c r="B9" s="2">
+        <v>56.2</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3">
-        <v>81.666666666666671</v>
+      <c r="B10" s="2">
+        <v>81.05</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3">
-        <v>70</v>
+      <c r="B11" s="2">
+        <v>69.75</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>59.666666666666664</v>
+      <c r="B12" s="2">
+        <v>66.550000000000011</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
-        <v>64</v>
+      <c r="B13" s="2">
+        <v>62.849999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3">
-        <v>55.333333333333336</v>
+      <c r="B14" s="2">
+        <v>54.95</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
-        <v>65</v>
+      <c r="B15" s="2">
+        <v>66.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>62</v>
-      </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>68</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>70</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>76</v>
-      </c>
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>78</v>
-      </c>
-      <c r="B34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>86</v>
-      </c>
-      <c r="B38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>88</v>
-      </c>
-      <c r="B39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>90</v>
-      </c>
-      <c r="B40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>92</v>
-      </c>
-      <c r="B41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>94</v>
-      </c>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>98</v>
-      </c>
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>100</v>
-      </c>
-      <c r="B45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>